<commit_message>
template raster uploaded to csc
</commit_message>
<xml_diff>
--- a/file_pointers_csc.xlsx
+++ b/file_pointers_csc.xlsx
@@ -8,24 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6480A6-E561-49B1-BDBC-48EDF7CC357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A161AEDA-0B4D-4C69-AA38-1D5296A8C4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="3705" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="4395" windowWidth="15990" windowHeight="11205" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -91,19 +86,29 @@
   </si>
   <si>
     <t>data/new_area/best_initial_zeta.p</t>
+  </si>
+  <si>
+    <t>data/new_area/new_area_dtm.tif</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -136,18 +141,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A9F55730-A72C-445A-B56E-E845830806C5}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{897EC50F-E97A-4367-BDF1-B7D9F79E2823}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +470,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,8 +575,8 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>